<commit_message>
adapted repetition handling order
</commit_message>
<xml_diff>
--- a/dialog1-future-self-activity.xlsx
+++ b/dialog1-future-self-activity.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24818"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leidenuniv1.sharepoint.com/sites/TeamAio/Shared Documents/General/Virtual Coach Dialogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nalbers1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1319" documentId="11_509B4261710A3368E50D86C241F188902C73F800" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF6A8A43-89F5-4881-93A7-5172E113D3FA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={1D5F984A-B538-4F8D-BB14-0850EDC40064}</author>
     <author>tc={4C9A13BB-D20D-4CA7-9F38-701E2EC686E1}</author>
@@ -56,9 +55,17 @@
     <author>tc={CBA2EF1A-AAC3-40E1-A3BF-D039E4CB63A7}</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{1D5F984A-B538-4F8D-BB14-0850EDC40064}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     We need at least 3 different formulations for each sentence since this dialog is going to be repeated. The formulations can just be slightly different, e.g. slightly different word order.
@@ -66,21 +73,39 @@
     It works best to use a new row for each sentence, when writing these different formulations (:
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{4C9A13BB-D20D-4CA7-9F38-701E2EC686E1}">
+    <comment ref="A11" authorId="1" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     If this takes 15 minutes and it is important that people do this dialog in 1 go, what if people do not do it in 1 go? E.g. what if they do not respond for say 30 minutes in the middle of the dialog? Do you then still let them continue the dialog as if nothing happened, or do they need to restart? At which point can we then assume that people will no longer get back to the dialog? It is also important for us to think about how we deal with people not completing dialogs and getting other messages in the mean time (e.g. to remind them of their scheduled PA activity). If we just have a single chat in NiceDay, then this would be very confusing, and probably not possible to continue the dialog after such an interruption.
 Reply:
     Great point! Issue #16 is about this topic, something we need to think about indeed. Let's brainstorm about the issue together and we'll alter the dialog accordingly. </t>
+        </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{05F931A5-B161-43FC-9555-BE3D9276AD56}">
+    <comment ref="A12" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Is it necessary to repeat this here (since it the VC already mentioned this at the beginning of the dialog)? Or maybe repeat it, but with a slightly different focus (e.g., Deze oefening helpt je doelen te stellen voor stoppen met roken en meer bewegen).
@@ -88,11 +113,20 @@
     We decided to repeat this because the generic rescheduling dialog happens in between.. Probably doesn't hurt to repeat this. We've added alternative formulations for more variation. 
 Reply:
     Agreed</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="3" shapeId="0" xr:uid="{A5D3429A-155E-4267-8200-A49305EB238E}">
+    <comment ref="A23" authorId="3" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Not so clear yet how people are supposed to choose 3 to 5 words as they cannot click on any words. Are they supposed to type all chosen words at once? Or do the words have numbers associated with them that the user can type? If users just type the words,  we have to do quite some processing since some words consist of multiple words, users may make typos, users may type other words in between such as "and", and we do not know in advance how many words the user will type (e.g. 3 or 5). The processing is necessary since it appears that you want to store just the single words that users selected. Just storing whatever the user typed would be easier.
@@ -101,19 +135,37 @@
 Reply:
     As discussed during the closing, the order of the words or whether there are typo's in there does not matter so much. I just want to be able to show the user their answer again. we only need to store what the user typed. 
 Resolved for now. </t>
+        </r>
       </text>
     </comment>
-    <comment ref="C24" authorId="4" shapeId="0" xr:uid="{36E234AB-0D9A-48D1-AE2C-C0C623D0FDCE}">
+    <comment ref="C24" authorId="4" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This needs a condition what to do when users do not pick the words but type something else. Also it might be good to say something like: 'typ de woorden achter elkaar, gescheiden door comma's'</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="5" shapeId="0" xr:uid="{D844C764-DA56-4806-86FE-BF5DB9BBEF57}">
+    <comment ref="A25" authorId="5" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This could sound a bit weird if they selected 'helpt mij ontspannen', 'moet ik doen' etc. "Roken is voor jou dus helpt mijn ontspannen, moet ik doen en hoort niet bij mij." is possibly not a very readable sentence. Maybe write something like "Deze woorden omschrijven jou als roker: ... "  
@@ -121,29 +173,56 @@
     Good point! Added you suggestion
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="6" shapeId="0" xr:uid="{F8CDE44F-7B6D-405C-AF3F-9DDA2015E2E0}">
+    <comment ref="A30" authorId="6" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     There are two VC utterances for the same condition. I think one of them should be when there are less than 5 words: 'kun je het in iets meer woorden opschrijven?'</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="7" shapeId="0" xr:uid="{19985CDD-C468-4CC7-A87B-53458642D567}">
+    <comment ref="A33" authorId="7" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Maybe you do not agree, but in my opinion sentences to explain what is coming (the sentence after that) can be left out. I think it is good to explain what is coming at the start of a dialog (so that the user knows what to expect), but I would not do that when you explain what is coming immediately after the sentence. This also makes the dialog shorter. So in this case, I would remove "Ik laat zo weer een lijst met woorden zien" and only say "Welke woorden passen bij jou?"
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A46" authorId="8" shapeId="0" xr:uid="{A7414AA0-76B6-43A4-97AC-3219994D8B9A}">
+    <comment ref="A46" authorId="8" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Again the requirement to select multiple options. This is not so straightforward to do and we need to think about how we want to design that.
@@ -151,21 +230,39 @@
     Not sure I understand why this is not possible. The user can type multiple words in the chat right?
 Reply:
     I agree with Nele. The user can type multiple words in the chat but we have to specify how they have to do this. For example the user could now type ' ik zie mijzelf als een roker en teglijkertijd als een niet-roker' a computer has a hard time making sense out of this. Better to enforce 'roker, niet-roker'. Even better would be to say: pick roker (1) or niet-roker(2) and user has to just type a number.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A49" authorId="9" shapeId="0" xr:uid="{108D51D6-1FA0-439B-907D-6C26912BB93C}">
+    <comment ref="A49" authorId="9" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I would first add a short reaction here, to show that the VC understands / is listening. Something like "Oke. / Oke, bedankt voor je antwoord etc."
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A51" authorId="10" shapeId="0" xr:uid="{60313AD4-4292-4A96-A6CC-967E8929269E}">
+    <comment ref="A51" authorId="10" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     It says to retrieve answer from line 39, is that correct? Line 39 has a free text response for why they chose the words for moving more.
@@ -173,49 +270,94 @@
     Line numbers still change due to editing. We need to check this at the end
 Reply:
     Better to not use line numbers!</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A53" authorId="11" shapeId="0" xr:uid="{C2569E76-62B6-49FD-A8B2-E8E0DF3C3FB6}">
+    <comment ref="A53" authorId="11" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Line 41 does not have any answer
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="12" shapeId="0" xr:uid="{650CFA75-C65F-4B72-8C76-A63B016828E9}">
+    <comment ref="A72" authorId="12" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     First say something that you got the response from the user that he is "klaar". This kind of backchanneling humans always do, like "Ok", "Cool", or just nodding or smiling. The latter we can of course not do.
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A73" authorId="13" shapeId="0" xr:uid="{55C3F65E-A90D-492B-9964-5301C64894A9}">
+    <comment ref="A73" authorId="13" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Again, make sure not to have the exact same formulations for sentences multiple times in the dialog.
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A82" authorId="14" shapeId="0" xr:uid="{21BFC4FE-B381-44E6-B454-BA171470E3E4}">
+    <comment ref="A82" authorId="14" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Add "in vergelijking met hoe je jezelf nu ziet"/ "in vergelijking met hoe je nu bent"? The sentence becomes more difficult this way, but I expect that how question is now is a bit too abstract..</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A94" authorId="15" shapeId="0" xr:uid="{2171E042-4E26-4891-8E9A-51D7F5BAFACE}">
+    <comment ref="A94" authorId="15" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Maybe give some examples or ask some subquestions here? "Hoe ziet jouw leven eruit?" is a very broad question. They can think about where they live, work, family, health, hobbies etc. Not sure what is most relevant to think about, but maybe help them a little bit more.
@@ -223,55 +365,101 @@
     I'm afraid that giving more direction will steer their mental image too much. That's why we chose to leave it very broad and open. But we could discuss this together and with Veronica and Winnie. 
 Reply:
     I agree with Kristell. Also, this is already a lot of text.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A95" authorId="16" shapeId="0" xr:uid="{A45E5BDA-10D0-430F-ADD3-0F5691F87B3A}">
+    <comment ref="A95" authorId="16" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I think it is more logical to turn row 56 and 57 around? So first mention that they think about the person they will be and then motivate them to envision this the best they can. And then ask the question to help them with that (like "hoe zie je eruit")
 Reply:
     Goed one, resolved. Also resolved for the undesired FS.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A101" authorId="17" shapeId="0" xr:uid="{4B1E541C-C6D6-433C-8651-F1399F6E5A40}">
+    <comment ref="A101" authorId="17" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I would leave this out too. Or rephrase it in something like "Goed, je hebt nu een beeld van jezelf als je straks ... Vat dit beeld samen met 5 woorden."
 Reply:
     Goeie suggestie voor een formulering. Resolved.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A102" authorId="18" shapeId="0" xr:uid="{8BF10B56-1E9D-4D33-A651-871188670CFB}">
+    <comment ref="A102" authorId="18" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Again, make sure not to have the exact same formulations for sentences multiple times in the dialog.
 Reply:
     Resolved</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A111" authorId="19" shapeId="0" xr:uid="{4A9D2639-C8EE-4429-BEEF-C88EF373DEA6}">
+    <comment ref="A111" authorId="19" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Add "in vergelijking met hoe je jezelf nu ziet"/ "in vergelijking met hoe je nu bent"? The sentence becomes more difficult this way, but I expect that how question is now is a bit too abstract..</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A117" authorId="20" shapeId="0" xr:uid="{CBA2EF1A-AAC3-40E1-A3BF-D039E4CB63A7}">
+    <comment ref="A117" authorId="20" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is not de mental contrasting part right? Or is it? If it is, then I think that we can keep it, but just do this on another day (so summarize parts of step 1-3 and them let them do the mental contrasting). However, we could consider it as a nice-to-have dialog instead of must-have?
 Reply:
     Good one. Let's see if this dialog is necessary. Related to our action points.
 Resolved for now. </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -625,7 +813,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1290,15 +1478,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.7109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" style="12" customWidth="1"/>
@@ -1386,7 +1574,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="26.1">
+    <row r="11" spans="1:3" ht="25.5">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -1440,32 +1628,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="38.25">
+    <row r="19" spans="1:3" ht="39">
       <c r="A19" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="25.5">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:3" ht="38.25">
+      <c r="A21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="25.5">
+      <c r="A23" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="39">
-      <c r="A22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="134.25" customHeight="1">
@@ -1482,12 +1670,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24.95">
+    <row r="26" spans="1:3" ht="25.5">
       <c r="A26" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="51.95">
+    <row r="27" spans="1:3" ht="51">
       <c r="A27" s="11"/>
       <c r="B27" s="5" t="s">
         <v>34</v>
@@ -1511,7 +1699,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="37.5">
+    <row r="30" spans="1:3" ht="38.25">
       <c r="A30" s="10" t="s">
         <v>39</v>
       </c>
@@ -1519,7 +1707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="26.1">
+    <row r="31" spans="1:3" ht="25.5">
       <c r="A31" s="10" t="s">
         <v>41</v>
       </c>
@@ -1532,27 +1720,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24.95">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:3" ht="49.5" customHeight="1">
+      <c r="A34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="25.5">
+      <c r="A36" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="49.5" customHeight="1">
-      <c r="A35" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="171" customHeight="1">
@@ -1569,12 +1757,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="38.450000000000003">
+    <row r="39" spans="1:3" ht="39">
       <c r="A39" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="51.95">
+    <row r="40" spans="1:3" ht="51">
       <c r="A40" s="8"/>
       <c r="B40" s="8" t="s">
         <v>50</v>
@@ -1583,7 +1771,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="24.95">
+    <row r="41" spans="1:3" ht="25.5">
       <c r="A41" s="8" t="s">
         <v>51</v>
       </c>
@@ -1605,7 +1793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="26.1">
+    <row r="44" spans="1:3" ht="25.5">
       <c r="A44" s="10" t="s">
         <v>41</v>
       </c>
@@ -1619,7 +1807,7 @@
       </c>
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="1:3" ht="24.95">
+    <row r="46" spans="1:3" ht="25.5">
       <c r="A46" s="8" t="s">
         <v>53</v>
       </c>
@@ -1657,7 +1845,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="26.1">
+    <row r="51" spans="1:8" ht="25.5">
       <c r="A51" s="8" t="s">
         <v>58</v>
       </c>
@@ -1674,7 +1862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="26.1">
+    <row r="53" spans="1:8" ht="25.5">
       <c r="A53" s="8" t="s">
         <v>60</v>
       </c>
@@ -1691,7 +1879,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="26.1">
+    <row r="55" spans="1:8" ht="25.5">
       <c r="A55" s="8" t="s">
         <v>62</v>
       </c>
@@ -1699,7 +1887,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="38.450000000000003">
+    <row r="56" spans="1:8" ht="39">
       <c r="A56" s="17" t="s">
         <v>63</v>
       </c>
@@ -1746,12 +1934,12 @@
       <c r="B61" s="1"/>
       <c r="C61" s="13"/>
     </row>
-    <row r="62" spans="1:8" ht="24.95">
+    <row r="62" spans="1:8" ht="25.5">
       <c r="A62" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="24.95">
+    <row r="63" spans="1:8" ht="25.5">
       <c r="A63" s="5" t="s">
         <v>70</v>
       </c>
@@ -1786,14 +1974,14 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" ht="37.5">
+    <row r="68" spans="1:3" ht="38.25">
       <c r="A68" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" ht="24.95">
+    <row r="69" spans="1:3" ht="25.5">
       <c r="A69" s="5" t="s">
         <v>76</v>
       </c>
@@ -1816,7 +2004,7 @@
       <c r="B71" s="10"/>
       <c r="C71" s="13"/>
     </row>
-    <row r="72" spans="1:3" ht="50.1">
+    <row r="72" spans="1:3" ht="51">
       <c r="A72" s="5" t="s">
         <v>80</v>
       </c>
@@ -1839,7 +2027,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="51.95">
+    <row r="75" spans="1:3" ht="51">
       <c r="A75" s="14" t="s">
         <v>83</v>
       </c>
@@ -1876,7 +2064,7 @@
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
     </row>
-    <row r="80" spans="1:3" ht="26.1">
+    <row r="80" spans="1:3" ht="25.5">
       <c r="A80" s="2" t="s">
         <v>88</v>
       </c>
@@ -1936,7 +2124,7 @@
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
     </row>
-    <row r="88" spans="1:3" ht="26.1">
+    <row r="88" spans="1:3" ht="25.5">
       <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
@@ -1957,12 +2145,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="24.95">
+    <row r="91" spans="1:3" ht="25.5">
       <c r="A91" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="24.95">
+    <row r="92" spans="1:3" ht="25.5">
       <c r="A92" s="5" t="s">
         <v>70</v>
       </c>
@@ -1987,7 +2175,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="37.5">
+    <row r="97" spans="1:3" ht="38.25">
       <c r="A97" s="5" t="s">
         <v>75</v>
       </c>
@@ -2013,7 +2201,7 @@
       <c r="B100" s="10"/>
       <c r="C100" s="9"/>
     </row>
-    <row r="101" spans="1:3" ht="50.1">
+    <row r="101" spans="1:3" ht="51">
       <c r="A101" s="5" t="s">
         <v>100</v>
       </c>
@@ -2034,13 +2222,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="51.95">
+    <row r="104" spans="1:3" ht="63.75">
       <c r="A104" s="9" t="s">
         <v>102</v>
       </c>
       <c r="C104" s="9"/>
     </row>
-    <row r="105" spans="1:3" ht="65.099999999999994">
+    <row r="105" spans="1:3" ht="63.75">
       <c r="A105" s="9" t="s">
         <v>103</v>
       </c>
@@ -2068,7 +2256,7 @@
       <c r="B108" s="22"/>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" ht="26.1">
+    <row r="109" spans="1:3" ht="25.5">
       <c r="A109" s="2" t="s">
         <v>106</v>
       </c>
@@ -2091,7 +2279,7 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:3" ht="37.5">
+    <row r="112" spans="1:3" ht="51">
       <c r="A112" s="10" t="s">
         <v>91</v>
       </c>
@@ -2128,7 +2316,7 @@
       <c r="B116" s="22"/>
       <c r="C116" s="22"/>
     </row>
-    <row r="117" spans="1:3" ht="26.1">
+    <row r="117" spans="1:3" ht="25.5">
       <c r="A117" s="2" t="s">
         <v>110</v>
       </c>
@@ -2176,6 +2364,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D8407203DC138A48A764EEEBAF3EF1CB" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8d5422cfa2882e8f2900ce6fdc5a2aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bb4f9b8-8294-49a6-848e-7a0f388aba11" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63eba17e0f4b5f97629da549ffbe3223" ns2:_="">
     <xsd:import namespace="9bb4f9b8-8294-49a6-848e-7a0f388aba11"/>
@@ -2347,23 +2544,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F12A30A-DE67-4C64-A6B4-ACD348DAD345}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F12A30A-DE67-4C64-A6B4-ACD348DAD345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D98B4A28-D371-4DB1-BE1D-553A1CD57B0E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{166120BF-77DD-4941-8F71-685073D8161F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{166120BF-77DD-4941-8F71-685073D8161F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D98B4A28-D371-4DB1-BE1D-553A1CD57B0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9bb4f9b8-8294-49a6-848e-7a0f388aba11"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>